<commit_message>
Update Unity Version to 2018.1.2f1
1. Update Unity Version to 2018.1.2f1
2. Add Xlsx excel to csv files
</commit_message>
<xml_diff>
--- a/Excel/UnitConfig.xlsx
+++ b/Excel/UnitConfig.xlsx
@@ -467,180 +467,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:I9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:I9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="3" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9">
+    <row r="1" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1">
+      <c r="A4" s="3">
+        <v>1001</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="F4" s="3">
+        <v>178</v>
+      </c>
+      <c r="G4" s="3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3">
+        <v>1002</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>179</v>
+      </c>
+      <c r="G5" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3">
+        <v>1003</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3">
         <v>2</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="F6" s="3">
+        <v>180</v>
+      </c>
+      <c r="G6" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3">
+        <v>1004</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3">
         <v>3</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="3:9">
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9">
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" s="3" customFormat="1">
-      <c r="C6" s="3">
-        <v>1001</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3">
-        <v>178</v>
-      </c>
-      <c r="I6" s="3">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9">
-      <c r="C7" s="3">
-        <v>1002</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>11</v>
+      <c r="F7" s="3">
+        <v>181</v>
       </c>
       <c r="G7" s="3">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3">
-        <v>179</v>
-      </c>
-      <c r="I7" s="3">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9">
-      <c r="C8" s="3">
-        <v>1003</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="3">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3">
-        <v>180</v>
-      </c>
-      <c r="I8" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9">
-      <c r="C9" s="3">
-        <v>1004</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="3">
-        <v>3</v>
-      </c>
-      <c r="H9" s="3">
-        <v>181</v>
-      </c>
-      <c r="I9" s="3">
         <v>71</v>
       </c>
     </row>

</xml_diff>